<commit_message>
New Pieces and Rulebook
</commit_message>
<xml_diff>
--- a/Kerd.xlsx
+++ b/Kerd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egeal\OneDrive\Belgeler\GitHub\Kerd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AE997A-4B1C-4D2F-8D7B-82B2A2845DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FBCA87-6260-4D45-9787-E46ADE9F4E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{50653107-51A8-4999-A1A6-327513E1B716}"/>
+    <workbookView xWindow="-4125" yWindow="2415" windowWidth="9045" windowHeight="11160" xr2:uid="{50653107-51A8-4999-A1A6-327513E1B716}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Piece Setup" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,8 +84,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="0"/>
+      <name val="Bahnschrift"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -81,6 +136,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA14A0F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -109,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -129,6 +190,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,6 +206,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA14A0F"/>
       <color rgb="FF90EB89"/>
       <color rgb="FF1ACC51"/>
       <color rgb="FF88D0F0"/>
@@ -145,7 +215,6 @@
       <color rgb="FFF4B184"/>
       <color rgb="FFF3AA79"/>
       <color rgb="FFF19E65"/>
-      <color rgb="FFA14A0F"/>
     </mruColors>
   </colors>
   <extLst>
@@ -163,15 +232,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>153653</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>693965</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -233,16 +302,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>136072</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>649169</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>693965</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>156055</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>183267</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>669152</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>713946</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -257,7 +326,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="993322" y="1020536"/>
+          <a:off x="1592132" y="1619344"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -303,15 +372,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>217714</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>730811</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>721179</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -327,7 +396,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1932214" y="1047750"/>
+          <a:off x="2518368" y="1626577"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -373,16 +442,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200133</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>713230</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>721179</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>199824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>693247</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>730503</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -397,7 +466,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2771883" y="1047750"/>
+          <a:off x="3345381" y="1635901"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -443,16 +512,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>204107</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>193639</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>717204</xdr:colOff>
+      <xdr:rowOff>181082</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>706737</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>680358</xdr:rowOff>
+      <xdr:rowOff>711761</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -467,8 +536,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1918607" y="8722179"/>
-          <a:ext cx="513097" cy="530679"/>
+          <a:off x="5952601" y="8533774"/>
+          <a:ext cx="513098" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -514,15 +583,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>186526</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
+      <xdr:colOff>225157</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>120371</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>699623</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>680358</xdr:rowOff>
+      <xdr:colOff>738254</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>651050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -537,7 +606,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2758276" y="8722179"/>
+          <a:off x="2525811" y="9337640"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -583,15 +652,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>676383</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>721179</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -607,7 +676,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3592286" y="1047750"/>
+          <a:off x="4193094" y="1626577"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -654,22 +723,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>145707</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>217714</xdr:rowOff>
+      <xdr:colOff>193641</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>237604</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>658804</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>748393</xdr:rowOff>
+      <xdr:colOff>706738</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>768283</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="Oval 50">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32C52910-6EE1-4A1A-92E0-5243C11E6D05}"/>
+        <xdr:cNvPr id="52" name="Oval 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B01396B-30F2-42D0-9602-7773DBA07F19}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -677,14 +746,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3574707" y="1932214"/>
+          <a:off x="3358872" y="9454873"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="bg1"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -723,23 +792,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>149679</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>662776</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>680358</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>192641</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>107020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>705738</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>637699</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="Oval 51">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B01396B-30F2-42D0-9602-7773DBA07F19}"/>
+        <xdr:cNvPr id="54" name="Oval 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75934744-1A65-4D37-956C-5088E8BBAC60}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -747,14 +816,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3578679" y="8722179"/>
+          <a:off x="5951603" y="2407674"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="bg1"/>
+          <a:schemeClr val="tx1"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -794,22 +863,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>149677</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>176892</xdr:rowOff>
+      <xdr:colOff>175011</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>662774</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>707571</xdr:rowOff>
+      <xdr:colOff>688108</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>693964</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="54" name="Oval 53">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75934744-1A65-4D37-956C-5088E8BBAC60}"/>
+        <xdr:cNvPr id="55" name="Oval 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE908C14-3084-431C-AFD1-542F79561882}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -817,7 +886,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5293177" y="1891392"/>
+          <a:off x="5069396" y="2463939"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -863,23 +932,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>145704</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>658801</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>693965</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>166576</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>141429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>679673</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>672108</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="55" name="Oval 54">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE908C14-3084-431C-AFD1-542F79561882}"/>
+        <xdr:cNvPr id="57" name="Oval 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{380B5013-095A-4CEB-AF09-BD565FC7E8AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -887,14 +956,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6146454" y="1020536"/>
+          <a:off x="6790114" y="9358698"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="bg1"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -933,23 +1002,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>132097</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>122465</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>645194</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>653144</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>178254</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>167368</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>691351</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>698047</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="57" name="Oval 56">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{380B5013-095A-4CEB-AF09-BD565FC7E8AE}"/>
+        <xdr:cNvPr id="58" name="Oval 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5CEAFD1-C160-4C88-972B-D41FDC77B978}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -957,14 +1026,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6132847" y="8694965"/>
+          <a:off x="7607754" y="1596118"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="bg1"/>
+          <a:schemeClr val="tx1"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -1003,23 +1072,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>149679</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>662776</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>707572</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>181389</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>179557</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>694486</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>710236</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="58" name="Oval 57">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5CEAFD1-C160-4C88-972B-D41FDC77B978}"/>
+        <xdr:cNvPr id="59" name="Oval 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A308FF0-8983-4A30-B039-8A5D6F28E0BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1027,7 +1096,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7007679" y="1034143"/>
+          <a:off x="8534081" y="1615634"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1074,22 +1143,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>132098</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:colOff>163284</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>209341</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>645195</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>707572</xdr:rowOff>
+      <xdr:colOff>676381</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>740020</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="59" name="Oval 58">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A308FF0-8983-4A30-B039-8A5D6F28E0BF}"/>
+        <xdr:cNvPr id="60" name="Oval 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D756EBC-D167-4435-B366-474B63C7E59B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1097,14 +1166,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7847348" y="1034143"/>
+          <a:off x="7651399" y="9426610"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="bg1"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -1143,23 +1212,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>136072</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>136072</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>649169</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>666751</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>156173</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>178987</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>669270</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>709666</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="Oval 59">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D756EBC-D167-4435-B366-474B63C7E59B}"/>
+        <xdr:cNvPr id="61" name="Oval 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FC82A79-F113-4842-BDF1-1916FA380756}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1167,7 +1236,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6994072" y="8708572"/>
+          <a:off x="8508865" y="9396256"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1213,23 +1282,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>118491</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>136072</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>631588</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>666751</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>159312</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>672409</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>693965</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="61" name="Oval 60">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FC82A79-F113-4842-BDF1-1916FA380756}"/>
+        <xdr:cNvPr id="63" name="Oval 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64E25554-4F6F-4766-8FD3-EB9B09CA677A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1237,14 +1306,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7833741" y="8708572"/>
+          <a:off x="9589062" y="1020536"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="bg1"/>
+          <a:schemeClr val="tx1"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -1283,23 +1352,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>176893</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>689990</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>693965</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>196247</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>148587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>709344</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>679266</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="62" name="Oval 61">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{689C0EBA-2805-4A00-9A49-9316E92E06FE}"/>
+        <xdr:cNvPr id="64" name="Oval 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7155DE6-C779-4906-BB19-4D38CC8D770E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1307,14 +1376,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8749393" y="1020536"/>
+          <a:off x="9426838" y="9379178"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="bg1"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -1353,23 +1422,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>159312</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>672409</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>693965</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>205082</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>148252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>718179</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>678931</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="63" name="Oval 62">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64E25554-4F6F-4766-8FD3-EB9B09CA677A}"/>
+        <xdr:cNvPr id="65" name="Oval 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C544FE79-08B5-41B4-A68B-70EFA3F21015}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1377,14 +1446,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9589062" y="1020536"/>
+          <a:off x="10286928" y="9365521"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="bg1"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -1423,23 +1492,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>122465</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>676383</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>653144</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>166806</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>123321</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>679903</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>654000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="64" name="Oval 63">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7155DE6-C779-4906-BB19-4D38CC8D770E}"/>
+        <xdr:cNvPr id="70" name="Oval 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55F96636-7620-4C1B-A6D3-9B2EF788B8AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1447,7 +1516,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8735786" y="8694965"/>
+          <a:off x="738306" y="9340590"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1493,23 +1562,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>145705</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>122465</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>658802</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>653144</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>157220</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>207248</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>670317</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>737927</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="65" name="Oval 64">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C544FE79-08B5-41B4-A68B-70EFA3F21015}"/>
+        <xdr:cNvPr id="71" name="Oval 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8166ED2-B5E3-4046-9FA5-70F0030610F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1517,7 +1586,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9575455" y="8694965"/>
+          <a:off x="1593297" y="9424517"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1563,23 +1632,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>204107</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>717204</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>693965</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>174597</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>214155</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>687694</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>744834</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="70" name="Oval 69">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55F96636-7620-4C1B-A6D3-9B2EF788B8AD}"/>
+        <xdr:cNvPr id="72" name="Oval 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2368111-B37F-43F2-BEAF-212AAF8B6812}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1587,14 +1656,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="204107" y="8735786"/>
+          <a:off x="6798135" y="1650232"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="bg1"/>
+          <a:schemeClr val="tx1"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -1633,23 +1702,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>186526</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>699623</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>693965</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>153137</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>134537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666234</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>674741</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="71" name="Oval 70">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8166ED2-B5E3-4046-9FA5-70F0030610F0}"/>
+        <xdr:cNvPr id="76" name="Oval 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB0674F8-8E06-4048-9673-724B44CFB394}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1657,8 +1726,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1043776" y="8735786"/>
-          <a:ext cx="513097" cy="530679"/>
+          <a:off x="4182945" y="9351806"/>
+          <a:ext cx="513097" cy="540204"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1703,23 +1772,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>134820</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>647917</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>683079</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>204625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>124941</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>721910</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>655620</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="72" name="Oval 71">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2368111-B37F-43F2-BEAF-212AAF8B6812}"/>
+        <xdr:cNvPr id="77" name="Oval 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F20E0700-FB3F-45BE-91F9-2DBA45D96C89}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1727,14 +1796,14 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4421070" y="1866900"/>
-          <a:ext cx="513097" cy="530679"/>
+          <a:off x="5099010" y="8477633"/>
+          <a:ext cx="517285" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="bg1"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -1773,365 +1842,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>166005</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>193221</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>679102</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>723900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="73" name="Oval 72">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FCC2AF0-3EFE-43E9-A68F-C2EEA3F7A0D5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6166755" y="1907721"/>
-          <a:ext cx="513097" cy="530679"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="3600" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>676383</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>707572</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="75" name="Oval 74">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F63AAD6E-3A88-4392-B513-F228E366DEEC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3592286" y="7892143"/>
-          <a:ext cx="513097" cy="530679"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="3600" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>145705</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>658802</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>707572</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="76" name="Oval 75">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB0674F8-8E06-4048-9673-724B44CFB394}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4431955" y="7892143"/>
-          <a:ext cx="513097" cy="530679"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="3600" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>703597</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>721179</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="77" name="Oval 76">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F20E0700-FB3F-45BE-91F9-2DBA45D96C89}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5334000" y="7905750"/>
-          <a:ext cx="513097" cy="530679"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="3600" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>172919</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>686016</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>721179</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="78" name="Oval 77">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1D720C4-E233-4048-B9E4-DB4B9C41B3DB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6173669" y="7905750"/>
-          <a:ext cx="513097" cy="530679"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-GB" sz="3600" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>136072</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>163285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>639536</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>693963</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2197,16 +1916,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>721178</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>145968</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>155863</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>649432</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>686541</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2221,7 +1940,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9593036" y="190500"/>
+          <a:off x="10242468" y="727363"/>
           <a:ext cx="503464" cy="530678"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2271,16 +1990,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>217714</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>136071</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>721178</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>666749</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>183078</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>686542</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>666750</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2295,7 +2014,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9647464" y="9565821"/>
+          <a:off x="10279578" y="10232572"/>
           <a:ext cx="503464" cy="530678"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2353,16 +2072,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>136071</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>122464</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>639535</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>653142</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>146251</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>181840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>649715</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>712518</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2377,7 +2096,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="136071" y="9552214"/>
+          <a:off x="717751" y="10263686"/>
           <a:ext cx="503464" cy="530678"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2424,6 +2143,1971 @@
             <a:t>R</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="3600" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>81032</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>60607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>753385</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>676931</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Isosceles Triangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31A2D8E5-F6E8-45F9-8FD4-959E91FD8609}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6704570" y="10142453"/>
+          <a:ext cx="672353" cy="616324"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>B</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>33125</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>60771</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>709664</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>677095</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Isosceles Triangle 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0053C625-A2C3-45F8-908D-3534D75322BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4062933" y="10142617"/>
+          <a:ext cx="676539" cy="616324"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>B</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>97283</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>148387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>773822</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>764711</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Isosceles Triangle 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04AEBE15-436A-461B-B42F-50EC03D22CD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6720821" y="719887"/>
+          <a:ext cx="676539" cy="616324"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>B</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>144814</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>115506</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>817167</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>731830</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="Isosceles Triangle 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7064C421-562E-4188-8622-9D8453006AB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4174622" y="687006"/>
+          <a:ext cx="672353" cy="616324"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>B</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>68096</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>45685</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>718037</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>729244</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Cross 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A40F269B-12DA-44EF-8851-6AF78D2C7661}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5827058" y="10127531"/>
+          <a:ext cx="649941" cy="683559"/>
+        </a:xfrm>
+        <a:prstGeom prst="plus">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 26724"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="3600" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>K</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="3600" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>118953</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>115508</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>768894</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>799067</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Cross 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4553953-F21E-4ECC-936D-80C58A974061}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5877915" y="687008"/>
+          <a:ext cx="649941" cy="683559"/>
+        </a:xfrm>
+        <a:prstGeom prst="plus">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 26724"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="3600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>K</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="3600" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>112521</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>153620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>695227</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>758737</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Chord 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C74E901-4C22-415A-9233-2C4A5DC1A2C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3277752" y="10235466"/>
+          <a:ext cx="582706" cy="605117"/>
+        </a:xfrm>
+        <a:prstGeom prst="chord">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 75687"/>
+            <a:gd name="adj2" fmla="val 15337109"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>H</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>143015</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>117149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>725721</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>722266</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Chord 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9286CF6-8925-4F41-9ADF-7540CB4441CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7631130" y="10198995"/>
+          <a:ext cx="582706" cy="605117"/>
+        </a:xfrm>
+        <a:prstGeom prst="chord">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 86445"/>
+            <a:gd name="adj2" fmla="val 15337109"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>H</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>140348</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>136353</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>723054</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>741470</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Chord 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FBC4176-B660-4BE9-BBB3-BE84D44FDA46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7628463" y="707853"/>
+          <a:ext cx="582706" cy="605117"/>
+        </a:xfrm>
+        <a:prstGeom prst="chord">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 86445"/>
+            <a:gd name="adj2" fmla="val 15337109"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>H</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>183265</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>118773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>765971</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>723890</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Chord 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7C851BF-7EF0-45F5-9986-4B8C00A0FD44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3348496" y="690273"/>
+          <a:ext cx="582706" cy="605117"/>
+        </a:xfrm>
+        <a:prstGeom prst="chord">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 86445"/>
+            <a:gd name="adj2" fmla="val 15337109"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>H</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19827</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>199981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>725796</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>816305</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Heart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0714FDB-F105-4787-9450-181110A90C82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4914212" y="771481"/>
+          <a:ext cx="705969" cy="616324"/>
+        </a:xfrm>
+        <a:prstGeom prst="heart">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1"/>
+            <a:t>Q</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>73112</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>145678</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>779081</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>762002</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Heart 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D329889-008A-40B6-B225-532D9615DD1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4967497" y="10227524"/>
+          <a:ext cx="705969" cy="616324"/>
+        </a:xfrm>
+        <a:prstGeom prst="heart">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Q</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>186191</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171535</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>699288</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>702214</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="Trapezoid 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07DC4BA9-F859-43C8-8902-B03357C8CF36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5080576" y="9388804"/>
+          <a:ext cx="513097" cy="530679"/>
+        </a:xfrm>
+        <a:prstGeom prst="trapezoid">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="4000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="4000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>187208</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>172318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>700305</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>702997</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="Trapezoid 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8C2089C-F0B6-4C22-9A6B-73AE922FC5DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5946170" y="9389587"/>
+          <a:ext cx="513097" cy="530679"/>
+        </a:xfrm>
+        <a:prstGeom prst="trapezoid">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="4000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="4000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171536</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>181793</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>684633</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>712472</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Trapezoid 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6427E647-0D8F-4862-99F3-1A925AB8A5D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5930498" y="1617870"/>
+          <a:ext cx="513097" cy="530679"/>
+        </a:xfrm>
+        <a:prstGeom prst="trapezoid">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="4000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="4000" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>169769</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>140375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>682866</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>671054</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="Trapezoid 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84EE0770-9335-4472-9343-E9F0E60D0C32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5064154" y="1576452"/>
+          <a:ext cx="513097" cy="530679"/>
+        </a:xfrm>
+        <a:prstGeom prst="trapezoid">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="4000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="4000" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>52287</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>175113</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>565384</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>705792</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="Oval 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65ED37EF-ABBC-4120-862A-9617FFE7B30E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9269556" y="1611190"/>
+          <a:ext cx="513097" cy="530679"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="3600" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123337</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>822850</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>777874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="84" name="Picture 83" descr="Al Sana Taş! - Harmoni Kocluk&amp;amp;Akademi">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{242630DC-FA54-40ED-9C77-F8998FF8130B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9340606" y="10177095"/>
+          <a:ext cx="699513" cy="682625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>87494</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>127133</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>787007</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>809758</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="90" name="Picture 89" descr="Al Sana Taş! - Harmoni Kocluk&amp;amp;Akademi">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27BBC34B-B464-4026-8A0F-93C4C67F55E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1523571" y="10208979"/>
+          <a:ext cx="699513" cy="682625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>108681</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808194</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>792531</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="91" name="Picture 90" descr="Al Sana Taş! - Harmoni Kocluk&amp;amp;Akademi">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A32D541E-9C38-41A3-B1F2-0462C53A73D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9325950" y="681406"/>
+          <a:ext cx="699513" cy="682625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>94020</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>139216</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>793533</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>821841</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="94" name="Picture 93" descr="Al Sana Taş! - Harmoni Kocluk&amp;amp;Akademi">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C906F2A9-D820-474F-8FFB-43EFBA2B4CF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1530097" y="710716"/>
+          <a:ext cx="699513" cy="682625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>131885</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>804238</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>792170</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="95" name="Flowchart: Merge 94">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7781978C-71BE-45B5-8A71-1AD1C6F5CA26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8484577" y="747346"/>
+          <a:ext cx="672353" cy="616324"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartMerge">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>S</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>73270</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>175846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>745623</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>792170</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="96" name="Flowchart: Merge 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D77C8656-C76D-4D57-9C2C-4687284D563F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2373924" y="747346"/>
+          <a:ext cx="672353" cy="616324"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartMerge">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>S</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>117231</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161193</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>789584</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>777517</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="97" name="Flowchart: Merge 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFACDB74-8427-4B71-893B-4A7E00508884}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2417885" y="10243039"/>
+          <a:ext cx="672353" cy="616324"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartMerge">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>S</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>73269</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>117231</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>745622</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>733555</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="98" name="Flowchart: Merge 97">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{847B43F3-9B0F-4701-9DF8-89E3F9EC43FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8425961" y="10199077"/>
+          <a:ext cx="672353" cy="616324"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartMerge">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="50000"/>
+              <a:lumOff val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="2800" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>S</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="2800" b="1">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -2733,104 +4417,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D27E80-28FA-45B9-8B42-2509C9C36B11}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="3"/>
+    <row r="1" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>12</v>
+      </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="6"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="6"/>
+      <c r="H2" s="2"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="4"/>
+      <c r="J2" s="6"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>11</v>
+      </c>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="5"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="3"/>
+      <c r="J3" s="5"/>
       <c r="K3" s="4"/>
       <c r="L3" s="3"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>10</v>
+      </c>
       <c r="B4" s="4"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="6"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="6"/>
       <c r="K4" s="3"/>
       <c r="L4" s="4"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A5" s="9">
+        <v>9</v>
+      </c>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="5"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="3"/>
+      <c r="J5" s="5"/>
       <c r="K5" s="4"/>
       <c r="L5" s="3"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="7"/>
+      <c r="T5" s="10"/>
     </row>
-    <row r="6" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="2"/>
+    <row r="6" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="1"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="2"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>7</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
@@ -2842,76 +4552,156 @@
       <c r="J7" s="1"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
+    <row r="8" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="2"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="4"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+    <row r="9" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>5</v>
+      </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="5"/>
+      <c r="H9" s="1"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="4"/>
       <c r="L9" s="3"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+    <row r="10" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>4</v>
+      </c>
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="6"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="2"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="4"/>
+      <c r="J10" s="6"/>
       <c r="K10" s="3"/>
       <c r="L10" s="4"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>3</v>
+      </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="5"/>
+      <c r="H11" s="1"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="5"/>
       <c r="K11" s="4"/>
       <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>2</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="4"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="2"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="4"/>
+      <c r="J12" s="6"/>
       <c r="K12" s="3"/>
       <c r="L12" s="4"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the board setup
The board now includes all the pieces in their correct starting positions.
</commit_message>
<xml_diff>
--- a/Kerd.xlsx
+++ b/Kerd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egeal\OneDrive\Belgeler\GitHub\Kerd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FBCA87-6260-4D45-9787-E46ADE9F4E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10058E55-59A3-4180-8644-B83D554F1C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4125" yWindow="2415" windowWidth="9045" windowHeight="11160" xr2:uid="{50653107-51A8-4999-A1A6-327513E1B716}"/>
+    <workbookView xWindow="24195" yWindow="4410" windowWidth="9045" windowHeight="11160" xr2:uid="{50653107-51A8-4999-A1A6-327513E1B716}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Piece Setup" sheetId="1" r:id="rId1"/>
@@ -445,13 +445,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>180150</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>199824</xdr:rowOff>
+      <xdr:rowOff>159003</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>693247</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>730503</xdr:rowOff>
+      <xdr:rowOff>689682</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -466,7 +466,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3345381" y="1635901"/>
+          <a:off x="3323400" y="1587753"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -512,16 +512,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>193639</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152818</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>181082</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>706737</xdr:colOff>
+      <xdr:rowOff>208297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>665916</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>711761</xdr:rowOff>
+      <xdr:rowOff>738976</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -536,7 +536,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5952601" y="8533774"/>
+          <a:off x="5010568" y="8495047"/>
           <a:ext cx="513098" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -792,16 +792,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>192641</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>165427</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>107020</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>705738</xdr:colOff>
+      <xdr:rowOff>175053</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>678524</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>637699</xdr:rowOff>
+      <xdr:rowOff>705732</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -816,7 +816,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5951603" y="2407674"/>
+          <a:off x="5023177" y="2461053"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -862,16 +862,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>175011</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>175010</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>163285</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>688108</xdr:colOff>
+      <xdr:rowOff>190498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>688107</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>693964</xdr:rowOff>
+      <xdr:rowOff>721177</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -886,7 +886,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5069396" y="2463939"/>
+          <a:off x="5890010" y="2476498"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -933,15 +933,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>166576</xdr:colOff>
+      <xdr:colOff>181230</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>141429</xdr:rowOff>
+      <xdr:rowOff>126775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>679673</xdr:colOff>
+      <xdr:colOff>694327</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>672108</xdr:rowOff>
+      <xdr:rowOff>657454</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -956,7 +956,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6790114" y="9358698"/>
+          <a:off x="6804768" y="9344044"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1003,15 +1003,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>178254</xdr:colOff>
+      <xdr:colOff>131152</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>167368</xdr:rowOff>
+      <xdr:rowOff>216563</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>691351</xdr:colOff>
+      <xdr:colOff>644249</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>698047</xdr:rowOff>
+      <xdr:rowOff>747242</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1026,7 +1026,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7607754" y="1596118"/>
+          <a:off x="7560652" y="1645313"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1145,13 +1145,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>163284</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>209341</xdr:rowOff>
+      <xdr:rowOff>150725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>676381</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>740020</xdr:rowOff>
+      <xdr:rowOff>681404</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1166,7 +1166,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7651399" y="9426610"/>
+          <a:off x="7651399" y="9367994"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1213,15 +1213,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>156173</xdr:colOff>
+      <xdr:colOff>170827</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>178987</xdr:rowOff>
+      <xdr:rowOff>193640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>669270</xdr:colOff>
+      <xdr:colOff>683924</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>709666</xdr:rowOff>
+      <xdr:rowOff>724319</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1236,7 +1236,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8508865" y="9396256"/>
+          <a:off x="8523519" y="9410909"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1656,7 +1656,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6798135" y="1650232"/>
+          <a:off x="6746847" y="1642905"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1772,16 +1772,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>204625</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>150196</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>124941</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>721910</xdr:colOff>
+      <xdr:rowOff>192976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>667481</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>655620</xdr:rowOff>
+      <xdr:rowOff>723655</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1796,7 +1796,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5099010" y="8477633"/>
+          <a:off x="5865196" y="8479726"/>
           <a:ext cx="517285" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1906,7 +1906,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="tr-TR" sz="3600" b="1"/>
-            <a:t>R</a:t>
+            <a:t>T</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="3600" b="1"/>
         </a:p>
@@ -1980,7 +1980,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="tr-TR" sz="3600" b="1"/>
-            <a:t>R</a:t>
+            <a:t>T</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="3600" b="1"/>
         </a:p>
@@ -1993,13 +1993,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>183078</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>136072</xdr:rowOff>
+      <xdr:rowOff>149679</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>686542</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>666750</xdr:rowOff>
+      <xdr:rowOff>680357</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2014,7 +2014,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10279578" y="10232572"/>
+          <a:off x="10184328" y="10150929"/>
           <a:ext cx="503464" cy="530678"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2058,7 +2058,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>R</a:t>
+            <a:t>T</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="3600" b="1">
             <a:solidFill>
@@ -2140,7 +2140,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>R</a:t>
+            <a:t>T</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="3600" b="1">
             <a:solidFill>
@@ -2238,15 +2238,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>33125</xdr:colOff>
+      <xdr:colOff>60339</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>60771</xdr:rowOff>
+      <xdr:rowOff>115200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>709664</xdr:colOff>
+      <xdr:colOff>736878</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>677095</xdr:rowOff>
+      <xdr:rowOff>731524</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2261,7 +2261,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4062933" y="10142617"/>
+          <a:off x="4060839" y="10116450"/>
           <a:ext cx="676539" cy="616324"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -2321,15 +2321,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>97283</xdr:colOff>
+      <xdr:colOff>110890</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>148387</xdr:rowOff>
+      <xdr:rowOff>121173</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>773822</xdr:colOff>
+      <xdr:colOff>787429</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>764711</xdr:rowOff>
+      <xdr:rowOff>737497</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2344,7 +2344,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6720821" y="719887"/>
+          <a:off x="6683140" y="692673"/>
           <a:ext cx="676539" cy="616324"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -2404,15 +2404,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>144814</xdr:colOff>
+      <xdr:colOff>76778</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>115506</xdr:rowOff>
+      <xdr:rowOff>88292</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>817167</xdr:colOff>
+      <xdr:colOff>749131</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>731830</xdr:rowOff>
+      <xdr:rowOff>704616</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2427,7 +2427,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4174622" y="687006"/>
+          <a:off x="4077278" y="659792"/>
           <a:ext cx="672353" cy="616324"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
@@ -2657,15 +2657,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>112521</xdr:colOff>
+      <xdr:colOff>139735</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>153620</xdr:rowOff>
+      <xdr:rowOff>153621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>695227</xdr:colOff>
+      <xdr:colOff>722441</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>758737</xdr:rowOff>
+      <xdr:rowOff>758738</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2680,7 +2680,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3277752" y="10235466"/>
+          <a:off x="3282985" y="10154871"/>
           <a:ext cx="582706" cy="605117"/>
         </a:xfrm>
         <a:prstGeom prst="chord">
@@ -2996,15 +2996,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>19827</xdr:colOff>
+      <xdr:colOff>74256</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>199981</xdr:rowOff>
+      <xdr:rowOff>145552</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>725796</xdr:colOff>
+      <xdr:colOff>780225</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>816305</xdr:rowOff>
+      <xdr:rowOff>761876</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3019,7 +3019,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4914212" y="771481"/>
+          <a:off x="4932006" y="717052"/>
           <a:ext cx="705969" cy="616324"/>
         </a:xfrm>
         <a:prstGeom prst="heart">
@@ -3257,7 +3257,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5946170" y="9389587"/>
+          <a:off x="5902208" y="9316318"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
@@ -3394,15 +3394,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>169769</xdr:colOff>
+      <xdr:colOff>183376</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>140375</xdr:rowOff>
+      <xdr:rowOff>181196</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>682866</xdr:colOff>
+      <xdr:colOff>696473</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>671054</xdr:rowOff>
+      <xdr:rowOff>711875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3417,7 +3417,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5064154" y="1576452"/>
+          <a:off x="5041126" y="1609946"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
@@ -3474,15 +3474,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>52287</xdr:colOff>
+      <xdr:colOff>147537</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>175113</xdr:rowOff>
+      <xdr:rowOff>202327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>565384</xdr:colOff>
+      <xdr:colOff>660634</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>705792</xdr:rowOff>
+      <xdr:rowOff>733006</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3497,7 +3497,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9269556" y="1611190"/>
+          <a:off x="9291537" y="1631077"/>
           <a:ext cx="513097" cy="530679"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3539,250 +3539,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>123337</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>822850</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>777874</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="84" name="Picture 83" descr="Al Sana Taş! - Harmoni Kocluk&amp;amp;Akademi">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{242630DC-FA54-40ED-9C77-F8998FF8130B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9340606" y="10177095"/>
-          <a:ext cx="699513" cy="682625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>87494</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>127133</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>787007</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>809758</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="90" name="Picture 89" descr="Al Sana Taş! - Harmoni Kocluk&amp;amp;Akademi">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27BBC34B-B464-4026-8A0F-93C4C67F55E7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1523571" y="10208979"/>
-          <a:ext cx="699513" cy="682625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>108681</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>109906</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>808194</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>792531</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="91" name="Picture 90" descr="Al Sana Taş! - Harmoni Kocluk&amp;amp;Akademi">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A32D541E-9C38-41A3-B1F2-0462C53A73D0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9325950" y="681406"/>
-          <a:ext cx="699513" cy="682625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>94020</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>139216</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>793533</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>821841</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="94" name="Picture 93" descr="Al Sana Taş! - Harmoni Kocluk&amp;amp;Akademi">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C906F2A9-D820-474F-8FFB-43EFBA2B4CF5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1530097" y="710716"/>
-          <a:ext cx="699513" cy="682625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -4037,15 +3793,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>73269</xdr:colOff>
+      <xdr:colOff>59665</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>117231</xdr:rowOff>
+      <xdr:rowOff>198876</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>745622</xdr:colOff>
+      <xdr:colOff>732018</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>733555</xdr:rowOff>
+      <xdr:rowOff>815200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4060,7 +3816,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8425961" y="10199077"/>
+          <a:off x="8346415" y="10200126"/>
           <a:ext cx="672353" cy="616324"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartMerge">
@@ -4110,6 +3866,354 @@
           <a:endParaRPr lang="en-GB" sz="2800" b="1">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>113083</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>193315</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>793440</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>751208</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Arrow: Curved Down 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6E07036-CB07-438D-85EA-AB72A7225D19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9257083" y="10194565"/>
+          <a:ext cx="680357" cy="557893"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedDownArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 39891"/>
+            <a:gd name="adj2" fmla="val 54659"/>
+            <a:gd name="adj3" fmla="val 26723"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="4000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>J</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="4000" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>108858</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>789215</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>734786</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Arrow: Curved Down 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94DDCB6F-0DFB-41D1-82D8-EF0585E42F1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1537608" y="10178143"/>
+          <a:ext cx="680357" cy="557893"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedDownArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 39891"/>
+            <a:gd name="adj2" fmla="val 54659"/>
+            <a:gd name="adj3" fmla="val 26723"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="4000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>J</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="4000" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>204107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>775608</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>762000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Arrow: Curved Down 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6607085D-5A51-4171-8885-DDAFB29A673D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9239251" y="775607"/>
+          <a:ext cx="680357" cy="557893"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedDownArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 39891"/>
+            <a:gd name="adj2" fmla="val 54659"/>
+            <a:gd name="adj3" fmla="val 26723"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="4000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>J</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="4000" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>136071</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>816428</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>748393</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="73" name="Arrow: Curved Down 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66401BB8-0893-4B06-AC4E-680E2A0719DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1564821" y="762000"/>
+          <a:ext cx="680357" cy="557893"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedDownArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 39891"/>
+            <a:gd name="adj2" fmla="val 54659"/>
+            <a:gd name="adj3" fmla="val 26723"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="4000" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>J</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="4000" b="1">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -4419,8 +4523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D27E80-28FA-45B9-8B42-2509C9C36B11}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>